<commit_message>
Update Total Address Growth Rate, simplified.xlsx
</commit_message>
<xml_diff>
--- a/Output/Total Address Growth Rate, simplified.xlsx
+++ b/Output/Total Address Growth Rate, simplified.xlsx
@@ -12,15 +12,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Time Period</t>
   </si>
   <si>
-    <t xml:space="preserve">OZ tracts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">non-OZ tracts</t>
+    <t xml:space="preserve">Contiguous not selected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contiguous selected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ineligible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIC not selected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIC selected</t>
   </si>
   <si>
     <t xml:space="preserve">2014-09</t>
@@ -401,148 +410,494 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>10897091</v>
+        <v>15803506</v>
       </c>
       <c r="C2" t="n">
-        <v>104812931</v>
+        <v>227030</v>
+      </c>
+      <c r="D2" t="n">
+        <v>55062798</v>
+      </c>
+      <c r="E2" t="n">
+        <v>33946627</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10670061</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>10971745</v>
+        <v>15960120</v>
       </c>
       <c r="C3" t="n">
-        <v>105807137</v>
+        <v>230742</v>
+      </c>
+      <c r="D3" t="n">
+        <v>55712041</v>
+      </c>
+      <c r="E3" t="n">
+        <v>34134976</v>
+      </c>
+      <c r="F3" t="n">
+        <v>10741003</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>11041469</v>
+        <v>16110051</v>
       </c>
       <c r="C4" t="n">
-        <v>106802433</v>
+        <v>233418</v>
+      </c>
+      <c r="D4" t="n">
+        <v>56370128</v>
+      </c>
+      <c r="E4" t="n">
+        <v>34322254</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10808051</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>11112862</v>
+        <v>16259861</v>
       </c>
       <c r="C5" t="n">
-        <v>107853741</v>
+        <v>236255</v>
+      </c>
+      <c r="D5" t="n">
+        <v>57078682</v>
+      </c>
+      <c r="E5" t="n">
+        <v>34515198</v>
+      </c>
+      <c r="F5" t="n">
+        <v>10876607</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B6" t="n">
-        <v>11195482</v>
+        <v>16437369</v>
       </c>
       <c r="C6" t="n">
-        <v>108974130</v>
+        <v>238980</v>
+      </c>
+      <c r="D6" t="n">
+        <v>57816819</v>
+      </c>
+      <c r="E6" t="n">
+        <v>34719942</v>
+      </c>
+      <c r="F6" t="n">
+        <v>10956502</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B7" t="n">
-        <v>11282221</v>
+        <v>16616200</v>
       </c>
       <c r="C7" t="n">
-        <v>110146363</v>
+        <v>241444</v>
+      </c>
+      <c r="D7" t="n">
+        <v>58582032</v>
+      </c>
+      <c r="E7" t="n">
+        <v>34948131</v>
+      </c>
+      <c r="F7" t="n">
+        <v>11040777</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B8" t="n">
-        <v>11364760</v>
+        <v>16792486</v>
       </c>
       <c r="C8" t="n">
-        <v>111252080</v>
+        <v>244689</v>
+      </c>
+      <c r="D8" t="n">
+        <v>59313397</v>
+      </c>
+      <c r="E8" t="n">
+        <v>35146197</v>
+      </c>
+      <c r="F8" t="n">
+        <v>11120071</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B9" t="n">
-        <v>11477870</v>
+        <v>16994655</v>
       </c>
       <c r="C9" t="n">
-        <v>112566200</v>
+        <v>248863</v>
+      </c>
+      <c r="D9" t="n">
+        <v>60178302</v>
+      </c>
+      <c r="E9" t="n">
+        <v>35393243</v>
+      </c>
+      <c r="F9" t="n">
+        <v>11229007</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B10" t="n">
-        <v>11621567</v>
+        <v>17216365</v>
       </c>
       <c r="C10" t="n">
-        <v>113963649</v>
+        <v>253408</v>
+      </c>
+      <c r="D10" t="n">
+        <v>61059978</v>
+      </c>
+      <c r="E10" t="n">
+        <v>35687306</v>
+      </c>
+      <c r="F10" t="n">
+        <v>11368159</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B11" t="n">
-        <v>11742219</v>
+        <v>17394800</v>
       </c>
       <c r="C11" t="n">
-        <v>115079534</v>
+        <v>256691</v>
+      </c>
+      <c r="D11" t="n">
+        <v>61765087</v>
+      </c>
+      <c r="E11" t="n">
+        <v>35919647</v>
+      </c>
+      <c r="F11" t="n">
+        <v>11485528</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B12" t="n">
-        <v>11956013</v>
+        <v>17680903</v>
       </c>
       <c r="C12" t="n">
-        <v>116766042</v>
+        <v>263739</v>
+      </c>
+      <c r="D12" t="n">
+        <v>62780406</v>
+      </c>
+      <c r="E12" t="n">
+        <v>36304733</v>
+      </c>
+      <c r="F12" t="n">
+        <v>11692274</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B13" t="n">
-        <v>0.697077844876403</v>
+        <v>15803506</v>
       </c>
       <c r="C13" t="n">
-        <v>0.997614724337003</v>
+        <v>227030</v>
+      </c>
+      <c r="D13" t="n">
+        <v>55062798</v>
+      </c>
+      <c r="E13" t="n">
+        <v>33946627</v>
+      </c>
+      <c r="F13" t="n">
+        <v>10670061</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="n">
+        <v>15960120</v>
+      </c>
+      <c r="C14" t="n">
+        <v>230742</v>
+      </c>
+      <c r="D14" t="n">
+        <v>55712041</v>
+      </c>
+      <c r="E14" t="n">
+        <v>34134976</v>
+      </c>
+      <c r="F14" t="n">
+        <v>10741003</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="n">
+        <v>16110051</v>
+      </c>
+      <c r="C15" t="n">
+        <v>233418</v>
+      </c>
+      <c r="D15" t="n">
+        <v>56370128</v>
+      </c>
+      <c r="E15" t="n">
+        <v>34322254</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10808051</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="n">
+        <v>16259861</v>
+      </c>
+      <c r="C16" t="n">
+        <v>236255</v>
+      </c>
+      <c r="D16" t="n">
+        <v>57078682</v>
+      </c>
+      <c r="E16" t="n">
+        <v>34515198</v>
+      </c>
+      <c r="F16" t="n">
+        <v>10876607</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16437369</v>
+      </c>
+      <c r="C17" t="n">
+        <v>238980</v>
+      </c>
+      <c r="D17" t="n">
+        <v>57816819</v>
+      </c>
+      <c r="E17" t="n">
+        <v>34719942</v>
+      </c>
+      <c r="F17" t="n">
+        <v>10956502</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="n">
+        <v>16616200</v>
+      </c>
+      <c r="C18" t="n">
+        <v>241444</v>
+      </c>
+      <c r="D18" t="n">
+        <v>58582032</v>
+      </c>
+      <c r="E18" t="n">
+        <v>34948131</v>
+      </c>
+      <c r="F18" t="n">
+        <v>11040777</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="n">
+        <v>16792486</v>
+      </c>
+      <c r="C19" t="n">
+        <v>244689</v>
+      </c>
+      <c r="D19" t="n">
+        <v>59313397</v>
+      </c>
+      <c r="E19" t="n">
+        <v>35146197</v>
+      </c>
+      <c r="F19" t="n">
+        <v>11120071</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="n">
+        <v>16994655</v>
+      </c>
+      <c r="C20" t="n">
+        <v>248863</v>
+      </c>
+      <c r="D20" t="n">
+        <v>60178302</v>
+      </c>
+      <c r="E20" t="n">
+        <v>35393243</v>
+      </c>
+      <c r="F20" t="n">
+        <v>11229007</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="n">
+        <v>17216365</v>
+      </c>
+      <c r="C21" t="n">
+        <v>253408</v>
+      </c>
+      <c r="D21" t="n">
+        <v>61059978</v>
+      </c>
+      <c r="E21" t="n">
+        <v>35687306</v>
+      </c>
+      <c r="F21" t="n">
+        <v>11368159</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="n">
-        <v>1.16754098889552</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1.17423823280432</v>
+      <c r="B22" t="n">
+        <v>17394800</v>
+      </c>
+      <c r="C22" t="n">
+        <v>256691</v>
+      </c>
+      <c r="D22" t="n">
+        <v>61765087</v>
+      </c>
+      <c r="E22" t="n">
+        <v>35919647</v>
+      </c>
+      <c r="F22" t="n">
+        <v>11485528</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="n">
+        <v>17680903</v>
+      </c>
+      <c r="C23" t="n">
+        <v>263739</v>
+      </c>
+      <c r="D23" t="n">
+        <v>62780406</v>
+      </c>
+      <c r="E23" t="n">
+        <v>36304733</v>
+      </c>
+      <c r="F23" t="n">
+        <v>11692274</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1.00799658051637</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1.2389285086471</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.24679939773407</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.583211899326659</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.685427091015054</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1.25012576919903</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1.7834789518827</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.3940735455782</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.764724052376205</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1.15390764023835</v>
       </c>
     </row>
   </sheetData>

</xml_diff>